<commit_message>
Working on procuring list of local and billing addresses
</commit_message>
<xml_diff>
--- a/HAWK/docs/Bodies of Water.xlsx
+++ b/HAWK/docs/Bodies of Water.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HAWK\HAWK\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DE2023-CF07-4202-9A50-B2F339A92107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421E1CDF-9DE9-48A1-BA14-BE7A1059A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B3567775-FEFF-4B4F-8A79-4701E423C0C9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="91">
   <si>
     <t>Bodies of Water in the Cobbossee Watershed for Data Collection</t>
   </si>
@@ -162,42 +162,9 @@
     <t>https://www.westgardinermaine.org/</t>
   </si>
   <si>
-    <t>Body of Water 1</t>
-  </si>
-  <si>
-    <t>Body of Water 2</t>
-  </si>
-  <si>
-    <t>Body of Water 3</t>
-  </si>
-  <si>
-    <t>Body of Water 4</t>
-  </si>
-  <si>
-    <t>Cobboseecontee Lake</t>
-  </si>
-  <si>
     <t>Cochnewagon Lake</t>
   </si>
   <si>
-    <t>Cobboseecontee Stream</t>
-  </si>
-  <si>
-    <t>Body of Water 5</t>
-  </si>
-  <si>
-    <t>Body of Water 6</t>
-  </si>
-  <si>
-    <t>Body of Water 7</t>
-  </si>
-  <si>
-    <t>Body of Water 8</t>
-  </si>
-  <si>
-    <t>Body of Water 9</t>
-  </si>
-  <si>
     <t>Zip 1</t>
   </si>
   <si>
@@ -316,13 +283,28 @@
   </si>
   <si>
     <t>Mallard Pond</t>
+  </si>
+  <si>
+    <t>https://www.farmingdalemaine.org/</t>
+  </si>
+  <si>
+    <t>Tax Book Obtained?</t>
+  </si>
+  <si>
+    <t>Tax Book Extracted?</t>
+  </si>
+  <si>
+    <t>Nancy's Bog</t>
+  </si>
+  <si>
+    <t>Kezar Pond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +316,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -356,16 +346,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -678,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DAD510D-B361-4AD3-9A61-A94E7265AC13}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -713,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -739,7 +732,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -750,7 +743,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -758,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -769,7 +768,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -779,13 +781,16 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
       <c r="D8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -793,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
@@ -827,7 +832,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -838,7 +843,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
@@ -849,7 +854,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -857,21 +862,21 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
         <v>81</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -879,7 +884,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
@@ -887,7 +892,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
         <v>28</v>
@@ -895,23 +900,23 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
         <v>36</v>
@@ -919,458 +924,388 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" t="s">
-        <v>83</v>
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>31</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="D33" t="s">
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="3">
+        <v>11735</v>
+      </c>
+      <c r="E39" s="3">
+        <v>11737</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
-        <v>49</v>
-      </c>
-      <c r="I39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G41" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" t="s">
-        <v>49</v>
-      </c>
-      <c r="I41" t="s">
-        <v>50</v>
-      </c>
-      <c r="J41" t="s">
-        <v>10</v>
-      </c>
-      <c r="K41" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" t="s">
-        <v>41</v>
-      </c>
-      <c r="G43" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F45" t="s">
-        <v>43</v>
-      </c>
-      <c r="G45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F46" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" t="s">
-        <v>49</v>
-      </c>
-      <c r="H46" t="s">
-        <v>51</v>
-      </c>
-      <c r="I46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="F49" t="s">
         <v>35</v>
       </c>
-      <c r="G47" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J47" t="s">
-        <v>15</v>
-      </c>
-      <c r="K47" t="s">
-        <v>21</v>
-      </c>
-      <c r="L47" t="s">
-        <v>20</v>
-      </c>
-      <c r="M47" t="s">
-        <v>17</v>
-      </c>
-      <c r="N47" t="s">
-        <v>19</v>
-      </c>
-      <c r="O47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="3">
-        <v>11735</v>
-      </c>
-      <c r="E48" s="3">
-        <v>11737</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H35">
-    <sortCondition ref="A35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H36">
+    <sortCondition ref="A4:A36"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F39" r:id="rId1" xr:uid="{01D69C8D-A049-4FA6-B001-DA731EF6498B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last commit - recoding in C#
</commit_message>
<xml_diff>
--- a/HAWK/docs/Bodies of Water.xlsx
+++ b/HAWK/docs/Bodies of Water.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HAWK\HAWK\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421E1CDF-9DE9-48A1-BA14-BE7A1059A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC31CFB7-9D99-4B9E-AA3A-6223B6A09B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B3567775-FEFF-4B4F-8A79-4701E423C0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="92">
   <si>
     <t>Bodies of Water in the Cobbossee Watershed for Data Collection</t>
   </si>
@@ -201,9 +210,6 @@
     <t>04357</t>
   </si>
   <si>
-    <t>04284</t>
-  </si>
-  <si>
     <t>04364</t>
   </si>
   <si>
@@ -298,6 +304,12 @@
   </si>
   <si>
     <t>Kezar Pond</t>
+  </si>
+  <si>
+    <t>List of Billing/Local Compiled?</t>
+  </si>
+  <si>
+    <t>N/A (No addresses)</t>
   </si>
 </sst>
 </file>
@@ -671,28 +683,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DAD510D-B361-4AD3-9A61-A94E7265AC13}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="5" width="25.41796875" customWidth="1"/>
-    <col min="6" max="6" width="36.15625" customWidth="1"/>
-    <col min="7" max="7" width="23.68359375" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="22.578125" customWidth="1"/>
-    <col min="10" max="10" width="15.578125" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="20.83984375" customWidth="1"/>
-    <col min="13" max="13" width="16.578125" customWidth="1"/>
-    <col min="14" max="14" width="20.578125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="1" max="6" width="25.41796875" customWidth="1"/>
+    <col min="7" max="7" width="36.15625" customWidth="1"/>
+    <col min="8" max="8" width="23.68359375" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="22.578125" customWidth="1"/>
+    <col min="11" max="11" width="15.578125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="20.83984375" customWidth="1"/>
+    <col min="14" max="14" width="16.578125" customWidth="1"/>
+    <col min="15" max="15" width="20.578125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,610 +712,666 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
         <v>30</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>76</v>
       </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
       <c r="B29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>24</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>23</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>22</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>36</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>31</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
         <v>26</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>29</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>36</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="3">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="3">
         <v>11735</v>
       </c>
-      <c r="E39" s="3">
+      <c r="F39" s="3">
         <v>11737</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" t="s">
+      <c r="F41" s="3"/>
+      <c r="G41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" t="s">
+      <c r="F42" s="3"/>
+      <c r="G42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" t="s">
+      <c r="F45" s="3"/>
+      <c r="G45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" t="s">
+      <c r="F46" s="3"/>
+      <c r="G46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="F47" s="3"/>
+      <c r="G47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I36">
     <sortCondition ref="A4:A36"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F39" r:id="rId1" xr:uid="{01D69C8D-A049-4FA6-B001-DA731EF6498B}"/>
+    <hyperlink ref="G39" r:id="rId1" xr:uid="{01D69C8D-A049-4FA6-B001-DA731EF6498B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>